<commit_message>
final changes before i jettison this project
</commit_message>
<xml_diff>
--- a/data/country data.xlsx
+++ b/data/country data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gilad\Documents\Python Scripts\The NUFORC Vitrine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gilad\Documents\Tableau\The NUFORC Vitrine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF54E8F-CCA3-4C81-BC77-F042AFC22D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B213D1F-9A24-4179-BDD6-550BC9FC66D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pop" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="545">
   <si>
     <t>AD</t>
   </si>
@@ -1632,9 +1632,6 @@
   </si>
   <si>
     <t>East Asia &amp; Pacific (excluding high income)</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
   </si>
   <si>
     <t>Curacao</t>
@@ -2502,8 +2499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3DC52A-43AA-485D-84D0-E186A19E6495}">
   <dimension ref="A1:BF262"/>
   <sheetViews>
-    <sheetView topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="A247" sqref="A247"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,7 +2510,7 @@
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B1" s="1">
         <v>1960</v>
@@ -3569,7 +3566,7 @@
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B7">
         <v>92490932</v>
@@ -8673,7 +8670,7 @@
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B36">
         <v>91401583</v>
@@ -9025,7 +9022,7 @@
     </row>
     <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B38">
         <v>109420</v>
@@ -10961,7 +10958,7 @@
     </row>
     <row r="49" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B49">
         <v>4198307</v>
@@ -11313,7 +11310,7 @@
     </row>
     <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B51">
         <v>124826</v>
@@ -11841,7 +11838,7 @@
     </row>
     <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>537</v>
+        <v>111</v>
       </c>
       <c r="B54">
         <v>9602006</v>
@@ -29769,7 +29766,7 @@
     </row>
     <row r="156" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B156">
         <v>1488667</v>
@@ -48315,7 +48312,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -48324,10 +48323,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>